<commit_message>
file modified, step 5(div_cw) div_po updated
</commit_message>
<xml_diff>
--- a/test_dsd.xlsx
+++ b/test_dsd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\dummyRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924E45F0-A784-4CBD-954F-89F94AB8F1DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7EE70-A1A8-4094-87F5-5A7750A5CA1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="6915" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
   <si>
     <t>Revision History</t>
   </si>
@@ -184,6 +184,39 @@
   </si>
   <si>
     <t>rishi</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>college</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>Step 5</t>
+  </si>
+  <si>
+    <t>PQRS</t>
+  </si>
+  <si>
+    <t>div_po updaed and div_cw:step 5 added</t>
   </si>
 </sst>
 </file>
@@ -193,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +278,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -260,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -353,13 +391,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -386,6 +459,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -674,8 +754,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:E3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A2:E3" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:E4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A2:E4" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version " dataDxfId="3"/>
@@ -1008,13 +1088,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -1023,7 +1103,7 @@
     <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1112,7 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
@@ -1049,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="13">
         <v>43354</v>
       </c>
@@ -1063,6 +1143,23 @@
         <v>53</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="17">
+        <v>43354</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1080,13 +1177,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:B53"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -1104,17 +1201,17 @@
     <col min="16" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1245,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -1165,7 +1262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1182,7 +1279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1199,7 +1296,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1216,7 +1313,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1233,13 +1330,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1256,7 +1353,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1269,7 +1366,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1282,7 +1379,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1295,7 +1392,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1308,7 +1405,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -1321,7 +1418,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1334,12 +1431,12 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>11</v>
       </c>
@@ -1354,7 +1451,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1464,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1380,7 +1477,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1393,7 +1490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1406,7 +1503,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1419,7 +1516,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1432,17 +1529,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
@@ -1457,7 +1554,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
@@ -1470,7 +1567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
@@ -1483,7 +1580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1496,7 +1593,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
@@ -1509,7 +1606,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
@@ -1522,17 +1619,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="4" t="s">
         <v>11</v>
       </c>
@@ -1547,7 +1644,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>17</v>
       </c>
@@ -1562,7 +1659,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>17</v>
       </c>
@@ -1577,7 +1674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -1590,7 +1687,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
@@ -1603,7 +1700,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>18</v>
       </c>
@@ -1616,7 +1713,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>21</v>
       </c>
@@ -1629,7 +1726,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
@@ -1644,7 +1741,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>21</v>
       </c>
@@ -1657,17 +1754,17 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="4" t="s">
         <v>11</v>
       </c>
@@ -1682,7 +1779,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>17</v>
       </c>
@@ -1697,7 +1794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>17</v>
       </c>
@@ -1712,7 +1809,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +1822,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>18</v>
       </c>
@@ -1738,7 +1835,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>18</v>
       </c>
@@ -1751,7 +1848,7 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>21</v>
       </c>
@@ -1764,7 +1861,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>21</v>
       </c>
@@ -1779,7 +1876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>21</v>
       </c>
@@ -1791,6 +1888,141 @@
         <v>39</v>
       </c>
       <c r="E61" s="1"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1799,12 +2031,63 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDC3DBF-70E0-4324-AC9D-6CBCC10C4016}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
both div_cw and div_po updated
</commit_message>
<xml_diff>
--- a/test_dsd.xlsx
+++ b/test_dsd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\dummyRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C7EE70-A1A8-4094-87F5-5A7750A5CA1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F3FD65-C654-4378-935B-C38E7CCE5FAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="6915" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="67">
   <si>
     <t>Revision History</t>
   </si>
@@ -195,18 +195,12 @@
     <t>home</t>
   </si>
   <si>
-    <t>school</t>
-  </si>
-  <si>
     <t>office</t>
   </si>
   <si>
     <t>college</t>
   </si>
   <si>
-    <t>road</t>
-  </si>
-  <si>
     <t>0.2</t>
   </si>
   <si>
@@ -217,6 +211,18 @@
   </si>
   <si>
     <t>div_po updaed and div_cw:step 5 added</t>
+  </si>
+  <si>
+    <t>community home</t>
+  </si>
+  <si>
+    <t>primary school</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>div_cw and div_po updated</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -454,12 +460,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -467,6 +467,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -754,8 +761,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:E4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A2:E4" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:E5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A2:E5" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version " dataDxfId="3"/>
@@ -1088,10 +1095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1104,13 +1111,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
@@ -1147,19 +1154,36 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>43354</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="18" t="s">
+      <c r="B4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="15">
+        <v>43354</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1177,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1891,12 +1915,12 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1952,7 +1976,9 @@
         <v>19</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E69" s="1"/>
     </row>
     <row r="70" spans="1:5">
@@ -1963,66 +1989,10 @@
         <v>20</v>
       </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E74" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2034,57 +2004,60 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="A6" s="22">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>60</v>
+      <c r="B6" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
location cw added, div_cw updated
</commit_message>
<xml_diff>
--- a/test_dsd.xlsx
+++ b/test_dsd.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkatuwal\Desktop\dummyRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F3FD65-C654-4378-935B-C38E7CCE5FAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7619A9F9-3D66-400E-A0A7-B87806949E8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="11415" windowHeight="6915" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RivisionHistory" sheetId="4" r:id="rId1"/>
     <sheet name="div_cw" sheetId="19" r:id="rId2"/>
-    <sheet name="div_po" sheetId="20" r:id="rId3"/>
+    <sheet name="po_cw" sheetId="20" r:id="rId3"/>
+    <sheet name="location_cw" sheetId="21" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="73">
   <si>
     <t>Revision History</t>
   </si>
@@ -198,9 +199,6 @@
     <t>office</t>
   </si>
   <si>
-    <t>college</t>
-  </si>
-  <si>
     <t>0.2</t>
   </si>
   <si>
@@ -213,9 +211,6 @@
     <t>div_po updaed and div_cw:step 5 added</t>
   </si>
   <si>
-    <t>community home</t>
-  </si>
-  <si>
     <t>primary school</t>
   </si>
   <si>
@@ -223,6 +218,30 @@
   </si>
   <si>
     <t>div_cw and div_po updated</t>
+  </si>
+  <si>
+    <t>community center</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>makalu street</t>
+  </si>
+  <si>
+    <t>kanchan street</t>
+  </si>
+  <si>
+    <t>barun street</t>
+  </si>
+  <si>
+    <t>manasalu street</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>location_cw added. Div_cw updated</t>
   </si>
 </sst>
 </file>
@@ -438,7 +457,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -467,13 +486,19 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -761,8 +786,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:E5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A2:E5" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A2:E6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+  <autoFilter ref="A2:E6" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version " dataDxfId="3"/>
@@ -1095,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,13 +1136,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="12" t="s">
@@ -1158,10 +1183,10 @@
         <v>43354</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>53</v>
@@ -1175,15 +1200,32 @@
         <v>43354</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="26">
+        <v>43355</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1201,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1900,18 +1942,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E61" s="1"/>
+    <row r="63" spans="1:5">
+      <c r="A63" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3" t="s">
@@ -1919,23 +1953,33 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="3" t="s">
-        <v>61</v>
+      <c r="A65" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>44</v>
+      <c r="A66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1947,10 +1991,10 @@
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1964,33 +2008,18 @@
       <c r="D68" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E68" s="1"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1" t="s">
+      <c r="D69" s="1"/>
+      <c r="E69" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2001,10 +2030,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDC3DBF-70E0-4324-AC9D-6CBCC10C4016}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2013,51 +2042,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="22">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="22">
+      <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>64</v>
+      <c r="B3" s="20" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="22">
+      <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="22">
-        <v>4</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>58</v>
-      </c>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="22">
+      <c r="A6" s="20">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>63</v>
+      <c r="B6" s="20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="24">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FCA479-7FFE-4207-8DE2-79D48E85EB4D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="25">
+        <v>1002</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="25">
+        <v>1002</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="25">
+        <v>1003</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="25">
+        <v>1004</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>